<commit_message>
SK- Test Case Excel
</commit_message>
<xml_diff>
--- a/Documents/Test Protocol.xlsx
+++ b/Documents/Test Protocol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\Embedded System Diploma\Sprints\task\Sprint Three\MovingCarProject\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\Embedded System Diploma\Sprints\task\Sprint Four\Sprints_AirConditioningSystem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDECA34-4FDA-4E9E-9B84-970668B9A9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5665DBEB-DCEC-41BD-B610-ED0F06A04C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875C6DCD-AFAF-4A5F-9F21-083CA0FCED6F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -45,103 +45,169 @@
     <t>Pass / Fail</t>
   </si>
   <si>
-    <t>Double Press On Start Button</t>
-  </si>
-  <si>
-    <t>Press Start Button Two Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignore Second Press </t>
-  </si>
-  <si>
-    <t>Ignore Seconed Press</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Car Stop After Press Stop Button</t>
-  </si>
-  <si>
-    <t>Press Stop Button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Car Stop </t>
-  </si>
-  <si>
-    <t>Car Stop</t>
-  </si>
-  <si>
-    <t>Forward Led Turn On In Forward State</t>
-  </si>
-  <si>
     <t>pass</t>
   </si>
   <si>
-    <t>Rotate Led Turn On In Rotate State</t>
-  </si>
-  <si>
-    <t>Forward Led Turn On</t>
-  </si>
-  <si>
-    <t>Rotate Led Turn On</t>
-  </si>
-  <si>
-    <t>Stop Led Turn On In Rotate State</t>
-  </si>
-  <si>
-    <t>Stop Led Turn On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Short Side Led Turn On In Short Side State </t>
-  </si>
-  <si>
-    <t>Short Side Led Turn On</t>
-  </si>
-  <si>
-    <t>4 Motors On In Forward State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 Motors On </t>
-  </si>
-  <si>
-    <t>4 Motor Speed Is 50% In Forward State</t>
-  </si>
-  <si>
-    <t>4 motors speed is 50%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Motors In Left Side On </t>
-  </si>
-  <si>
-    <t>2 Motors In Right Side Off In Rotate State</t>
-  </si>
-  <si>
-    <t>2 Motors In Left Side On In Rotate State</t>
-  </si>
-  <si>
-    <t>2 Motors In Right Side Off</t>
-  </si>
-  <si>
-    <t>2 Motor Speed In Left Side Is 30% In Rotate State</t>
-  </si>
-  <si>
-    <t>2 motors In Left Side speed is 30%</t>
-  </si>
-  <si>
-    <t>4 Motors Off In Stop State</t>
-  </si>
-  <si>
-    <t>4 Motors Off</t>
-  </si>
-  <si>
-    <t>Idle State</t>
-  </si>
-  <si>
-    <t>All Component Is Off Except Stop Led</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop Led Turn On </t>
+    <t xml:space="preserve">Default Temprature </t>
+  </si>
+  <si>
+    <t>Intial Temprature = 20</t>
+  </si>
+  <si>
+    <t>Start With Temprature = 20</t>
+  </si>
+  <si>
+    <t>Temprature Increment</t>
+  </si>
+  <si>
+    <t>Incremant In Temprature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Decremant In Temprature</t>
+  </si>
+  <si>
+    <t>Temprature Decrement</t>
+  </si>
+  <si>
+    <t>Push The Set Button</t>
+  </si>
+  <si>
+    <t>Push The Incremant Button</t>
+  </si>
+  <si>
+    <t>Push The Decremant Button</t>
+  </si>
+  <si>
+    <t>Set New Temprature</t>
+  </si>
+  <si>
+    <t>User Can Set New Temprature</t>
+  </si>
+  <si>
+    <t>Push The Adjust Button</t>
+  </si>
+  <si>
+    <t>Push The Reset Button</t>
+  </si>
+  <si>
+    <t>Temprature Return To The Default = 20</t>
+  </si>
+  <si>
+    <t>Buzzer Turn On</t>
+  </si>
+  <si>
+    <t>Buzzer Turn Off</t>
+  </si>
+  <si>
+    <t>Temprature Exceed The Set Degree</t>
+  </si>
+  <si>
+    <t>Buzzer turn Off</t>
+  </si>
+  <si>
+    <t>Temprature Not Exceed The Set Degree</t>
+  </si>
+  <si>
+    <t>Buzzer Draw</t>
+  </si>
+  <si>
+    <t>Buzzer Char Draw On The Lcd When Buzzer Turn On</t>
+  </si>
+  <si>
+    <t>Buzzer Clear</t>
+  </si>
+  <si>
+    <t>Buzzer Char Clear From The Lcd When Buzzer Turn OFF</t>
+  </si>
+  <si>
+    <t>Buzzer Char Draw On Lcd</t>
+  </si>
+  <si>
+    <t>Buzzer Char Clear From Lcd</t>
+  </si>
+  <si>
+    <t>Buzzer Cleared</t>
+  </si>
+  <si>
+    <t>Buzzer Drawed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Temprature </t>
+  </si>
+  <si>
+    <t>Current Temprature Display On Lcd</t>
+  </si>
+  <si>
+    <t>Show Current Temprature On Lcd</t>
+  </si>
+  <si>
+    <t>Current Temprature Showed On Lcd</t>
+  </si>
+  <si>
+    <t>Incremant Button In Set Mode</t>
+  </si>
+  <si>
+    <t>Decremant Button In Set Mode</t>
+  </si>
+  <si>
+    <t>Set Button In Set Mode</t>
+  </si>
+  <si>
+    <t>Reset Button In Set Mode</t>
+  </si>
+  <si>
+    <t>Push Incremant Button</t>
+  </si>
+  <si>
+    <t>Push Decremant Button</t>
+  </si>
+  <si>
+    <t>Push Set Button</t>
+  </si>
+  <si>
+    <t>Push Reset Button</t>
+  </si>
+  <si>
+    <t>Error Massage On Lcd</t>
+  </si>
+  <si>
+    <t>Adjust Button In Set Mode</t>
+  </si>
+  <si>
+    <t>Incremant Button In Idle Mode</t>
+  </si>
+  <si>
+    <t>Decremant Button In Idle Mode</t>
+  </si>
+  <si>
+    <t>Set Button In Idle Mode</t>
+  </si>
+  <si>
+    <t>Reset Button In Idle Mode</t>
+  </si>
+  <si>
+    <t>Adjust Button In Idle Mode</t>
+  </si>
+  <si>
+    <t>Push Adjust Button</t>
+  </si>
+  <si>
+    <t>Turn To Set Mode</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Time Out</t>
+  </si>
+  <si>
+    <t>User Do Not Select Any Thing</t>
+  </si>
+  <si>
+    <t>Turn To Idle Mode With Default Temprature</t>
   </si>
 </sst>
 </file>
@@ -532,19 +598,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C123E326-AE56-4BD1-BFE1-3D77BAFFAE7E}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="42.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
@@ -573,19 +639,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -593,19 +659,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -613,19 +679,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -633,19 +699,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -653,19 +719,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -673,19 +739,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -693,19 +759,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -713,19 +779,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -733,19 +799,19 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -753,19 +819,19 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -773,19 +839,19 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -793,19 +859,19 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -813,19 +879,99 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>